<commit_message>
Final commit before the defense.
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -363,10 +363,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -642,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:E35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,11 +717,11 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>